<commit_message>
New TF on Simulink
</commit_message>
<xml_diff>
--- a/ExperimentalData/Feb15_data.xlsx
+++ b/ExperimentalData/Feb15_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,10 +42,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MeasuredTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>OffsetTime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -55,6 +51,22 @@
   </si>
   <si>
     <t>Angle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Radians</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Radians/ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeasuredTime(ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rad/s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -739,11 +751,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354914488"/>
-        <c:axId val="354909784"/>
+        <c:axId val="356600768"/>
+        <c:axId val="356600376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354914488"/>
+        <c:axId val="356600768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,12 +826,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354909784"/>
+        <c:crossAx val="356600376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="354909784"/>
+        <c:axId val="356600376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,7 +902,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354914488"/>
+        <c:crossAx val="356600768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -953,48 +965,17 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-TW"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1005,46 +986,16 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="6"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="6"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$O$5:$O$78</c:f>
@@ -1278,7 +1229,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$5:$Q$78</c:f>
+              <c:f>Sheet1!$T$5:$T$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="74"/>
@@ -1286,223 +1237,223 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.800000000000004</c:v>
+                  <c:v>79.689179505692323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>131.4</c:v>
+                  <c:v>142.5210325774882</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>203.4</c:v>
+                  <c:v>205.35288564928399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>279</c:v>
+                  <c:v>268.56785977639572</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>351.9</c:v>
+                  <c:v>312.66326885726988</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>400.5</c:v>
+                  <c:v>341.46120151517636</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>421.20000000000005</c:v>
+                  <c:v>383.72310268846763</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>502.20000000000005</c:v>
+                  <c:v>393.4296846414195</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>467.09999999999991</c:v>
+                  <c:v>391.23787581333363</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>496.80000000000018</c:v>
+                  <c:v>387.58486109985671</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>458.09999999999991</c:v>
+                  <c:v>325.22623947957931</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>361.79999999999973</c:v>
+                  <c:v>296.74391477929692</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>420.30000000000018</c:v>
+                  <c:v>319.62290475652725</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>422.10000000000036</c:v>
+                  <c:v>307.52701420140124</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>370.80000000000018</c:v>
+                  <c:v>307.87608005179959</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>423</c:v>
+                  <c:v>328.82003107573166</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>424.79999999999927</c:v>
+                  <c:v>302.89050910153748</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>373.5</c:v>
+                  <c:v>289.76179049599455</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>406.80000000000018</c:v>
+                  <c:v>318.69712141416483</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>414.90000000000055</c:v>
+                  <c:v>308.6956259614318</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>398.69999999999982</c:v>
+                  <c:v>308.01267103673894</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>413.10000000000036</c:v>
+                  <c:v>307.52701420140124</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>379.79999999999927</c:v>
+                  <c:v>306.82888250060245</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>411.30000000000109</c:v>
+                  <c:v>318.34805556376608</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>409.5</c:v>
+                  <c:v>289.91436553236224</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>354.59999999999854</c:v>
+                  <c:v>288.09073057387235</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>421.20000000000073</c:v>
+                  <c:v>314.84222028367304</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>408.60000000000036</c:v>
+                  <c:v>304.25641895092349</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>393.29999999999927</c:v>
+                  <c:v>308.01267103673837</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>418.5</c:v>
+                  <c:v>297.42686970399069</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>365.39999999999964</c:v>
+                  <c:v>296.11181820005891</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>432</c:v>
+                  <c:v>318.93994983183319</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>408.60000000000036</c:v>
+                  <c:v>299.1197260598795</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>396.89999999999964</c:v>
+                  <c:v>307.67119357439179</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>414</c:v>
+                  <c:v>297.42686970399001</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>369.90000000000146</c:v>
+                  <c:v>297.08539224164349</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>413.09999999999854</c:v>
+                  <c:v>313.47631043428606</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>413.10000000000036</c:v>
+                  <c:v>306.64676118735201</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>395.10000000000036</c:v>
+                  <c:v>308.69562596143214</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>418.5</c:v>
+                  <c:v>294.44075827793671</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>374.39999999999964</c:v>
+                  <c:v>295.44339423121022</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>421.20000000000073</c:v>
+                  <c:v>302.79605788854872</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>394.20000000000073</c:v>
+                  <c:v>309.03710342377872</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>420.29999999999927</c:v>
+                  <c:v>312.15399345243191</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>420.29999999999927</c:v>
+                  <c:v>302.79605788854872</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>395.10000000000218</c:v>
+                  <c:v>301.79342193527521</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>417.59999999999854</c:v>
+                  <c:v>293.77233430908808</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>373.5</c:v>
+                  <c:v>304.59789641327126</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>429.29999999999927</c:v>
+                  <c:v>314.84222028367117</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>400.5</c:v>
+                  <c:v>300.79078598200164</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>409.5</c:v>
+                  <c:v>306.13817773279305</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>414.90000000000146</c:v>
+                  <c:v>297.11445415333242</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>385.20000000000073</c:v>
+                  <c:v>291.57906816130344</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>416.69999999999709</c:v>
+                  <c:v>301.86607671449747</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>378.90000000000146</c:v>
+                  <c:v>306.64676118735082</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>429.29999999999927</c:v>
+                  <c:v>309.48029757703739</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>404.10000000000218</c:v>
+                  <c:v>301.45920995085027</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>407.69999999999709</c:v>
+                  <c:v>307.4750256704915</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>420.30000000000291</c:v>
+                  <c:v>296.11181820005891</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>377.09999999999854</c:v>
+                  <c:v>299.13425701572231</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>411.29999999999927</c:v>
+                  <c:v>300.84164432745951</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>381.60000000000218</c:v>
+                  <c:v>293.86981280454569</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>426.59999999999854</c:v>
+                  <c:v>311.48556948358322</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>412.20000000000073</c:v>
+                  <c:v>301.45920995084907</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>399.59999999999854</c:v>
+                  <c:v>311.42744566020411</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>421.20000000000073</c:v>
+                  <c:v>301.18312178980307</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>372.59999999999854</c:v>
+                  <c:v>292.76969835581571</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>415.80000000000291</c:v>
+                  <c:v>296.78024216890992</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>383.39999999999782</c:v>
+                  <c:v>298.78551407545336</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>421.20000000000073</c:v>
+                  <c:v>310.81714551473345</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>415.79999999999927</c:v>
+                  <c:v>300.12236201315426</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>392.40000000000146</c:v>
+                  <c:v>303.91494148857942</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>408.59999999999854</c:v>
+                  <c:v>295.44339423120903</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,11 +1468,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="401392312"/>
-        <c:axId val="401392704"/>
+        <c:axId val="356598024"/>
+        <c:axId val="356594496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="401392312"/>
+        <c:axId val="356598024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,15 +1543,16 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="401392704"/>
+        <c:crossAx val="356594496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="40"/>
+        <c:majorUnit val="50"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="401392704"/>
+        <c:axId val="356594496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="420"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1655,7 +1607,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="401392312"/>
+        <c:crossAx val="356598024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -2883,16 +2835,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3177,18 +3129,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:Q104"/>
+  <dimension ref="B4:T104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H52" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6:Q78"/>
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:17">
+    <row r="4" spans="2:20">
       <c r="F4" t="s">
         <v>2</v>
       </c>
@@ -3202,19 +3155,28 @@
         <v>3</v>
       </c>
       <c r="M4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" t="s">
         <v>4</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>6</v>
       </c>
-      <c r="O4" t="s">
-        <v>5</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:17">
+      <c r="R4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20">
       <c r="B5">
         <v>1</v>
       </c>
@@ -3258,10 +3220,22 @@
         <v>0</v>
       </c>
       <c r="Q5">
+        <f>P5*PI()/180</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:17">
+      <c r="R5">
+        <f>(Q6-Q5)/(M6-M5)</f>
+        <v>4.8694686130641804E-2</v>
+      </c>
+      <c r="S5">
+        <f>R5*1000</f>
+        <v>48.694686130641806</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20">
       <c r="B6">
         <v>1</v>
       </c>
@@ -3305,11 +3279,23 @@
         <v>55.800000000000004</v>
       </c>
       <c r="Q6">
-        <f>P6-P5</f>
-        <v>55.800000000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17">
+        <f t="shared" ref="Q6:Q69" si="6">P6*PI()/180</f>
+        <v>0.97389372261283602</v>
+      </c>
+      <c r="R6">
+        <f>(Q7-Q6)/(M7-M6)</f>
+        <v>0.10920774462478804</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6:S69" si="7">R6*1000</f>
+        <v>109.20774462478803</v>
+      </c>
+      <c r="T6">
+        <f>(Q7-Q5)/(M7-M5)*1000</f>
+        <v>79.689179505692323</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20">
       <c r="B7">
         <v>4</v>
       </c>
@@ -3353,11 +3339,23 @@
         <v>187.20000000000002</v>
       </c>
       <c r="Q7">
-        <f t="shared" ref="Q7:Q70" si="6">P7-P6</f>
-        <v>131.4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17">
+        <f t="shared" si="6"/>
+        <v>3.267256359733385</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R6:R69" si="8">(Q8-Q7)/(M8-M7)</f>
+        <v>0.17749998492782332</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="7"/>
+        <v>177.49998492782331</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ref="T7:T70" si="9">(Q8-Q6)/(M8-M6)*1000</f>
+        <v>142.5210325774882</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20">
       <c r="B8">
         <v>11</v>
       </c>
@@ -3402,10 +3400,22 @@
       </c>
       <c r="Q8">
         <f t="shared" si="6"/>
-        <v>203.4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17">
+        <v>6.8172560582898516</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="8"/>
+        <v>0.23187945776496088</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="7"/>
+        <v>231.87945776496088</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="9"/>
+        <v>205.35288564928399</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
       <c r="B9">
         <v>18</v>
       </c>
@@ -3450,10 +3460,22 @@
       </c>
       <c r="Q9">
         <f t="shared" si="6"/>
-        <v>279</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17">
+        <v>11.68672467135403</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="8"/>
+        <v>0.30709068188840238</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="7"/>
+        <v>307.0906818884024</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="9"/>
+        <v>268.56785977639572</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20">
       <c r="B10">
         <v>26</v>
       </c>
@@ -3498,10 +3520,22 @@
       </c>
       <c r="Q10">
         <f t="shared" si="6"/>
-        <v>351.9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17">
+        <v>17.828538309122077</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="8"/>
+        <v>0.31772925701078575</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="7"/>
+        <v>317.72925701078577</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="9"/>
+        <v>312.66326885726988</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20">
       <c r="B11">
         <v>34</v>
       </c>
@@ -3546,10 +3580,22 @@
       </c>
       <c r="Q11">
         <f t="shared" si="6"/>
-        <v>400.5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17">
+        <v>24.818581963359364</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="8"/>
+        <v>0.36756634047000603</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="7"/>
+        <v>367.56634047000603</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="9"/>
+        <v>341.46120151517636</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20">
       <c r="B12">
         <v>42</v>
       </c>
@@ -3594,10 +3640,22 @@
       </c>
       <c r="Q12">
         <f t="shared" si="6"/>
-        <v>421.20000000000005</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17">
+        <v>32.169908772759484</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="8"/>
+        <v>0.3984110683416146</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="7"/>
+        <v>398.41106834161462</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="9"/>
+        <v>383.72310268846763</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20">
       <c r="B13">
         <v>51</v>
       </c>
@@ -3642,10 +3700,22 @@
       </c>
       <c r="Q13">
         <f t="shared" si="6"/>
-        <v>502.20000000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17">
+        <v>40.934952276275006</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="8"/>
+        <v>0.38821109219359601</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="7"/>
+        <v>388.21109219359602</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="9"/>
+        <v>393.4296846414195</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20">
       <c r="B14">
         <v>60</v>
       </c>
@@ -3690,10 +3760,22 @@
       </c>
       <c r="Q14">
         <f t="shared" si="6"/>
-        <v>467.09999999999991</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17">
+        <v>49.087385212340521</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="8"/>
+        <v>0.39412707835944683</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="7"/>
+        <v>394.12707835944684</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="9"/>
+        <v>391.23787581333363</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20">
       <c r="B15">
         <v>69</v>
       </c>
@@ -3738,10 +3820,22 @@
       </c>
       <c r="Q15">
         <f t="shared" si="6"/>
-        <v>496.80000000000018</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17">
+        <v>57.758180936248351</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="8"/>
+        <v>0.38073110968504814</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="7"/>
+        <v>380.73110968504812</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="9"/>
+        <v>387.58486109985671</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20">
       <c r="B16">
         <v>78</v>
       </c>
@@ -3786,10 +3880,22 @@
       </c>
       <c r="Q16">
         <f t="shared" si="6"/>
-        <v>458.09999999999991</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17">
+        <v>65.753534239634362</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="8"/>
+        <v>0.27454787972675992</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="7"/>
+        <v>274.5478797267599</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="9"/>
+        <v>325.22623947957931</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20">
       <c r="B17">
         <v>87</v>
       </c>
@@ -3834,10 +3940,22 @@
       </c>
       <c r="Q17">
         <f t="shared" si="6"/>
-        <v>361.79999999999973</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17">
+        <v>72.068135473349841</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="8"/>
+        <v>0.31893994983183382</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="7"/>
+        <v>318.93994983183381</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="9"/>
+        <v>296.74391477929692</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20">
       <c r="B18">
         <v>97</v>
       </c>
@@ -3882,10 +4000,22 @@
       </c>
       <c r="Q18">
         <f t="shared" si="6"/>
-        <v>420.30000000000018</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17">
+        <v>79.403754319482019</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="8"/>
+        <v>0.32030585968122077</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="7"/>
+        <v>320.3058596812208</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="9"/>
+        <v>319.62290475652725</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20">
       <c r="B19">
         <v>106</v>
       </c>
@@ -3930,10 +4060,22 @@
       </c>
       <c r="Q19">
         <f t="shared" si="6"/>
-        <v>422.10000000000036</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17">
+        <v>86.770789092150096</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="8"/>
+        <v>0.29416731210886254</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="7"/>
+        <v>294.16731210886252</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="9"/>
+        <v>307.52701420140124</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20">
       <c r="B20">
         <v>116</v>
       </c>
@@ -3978,10 +4120,22 @@
       </c>
       <c r="Q20">
         <f t="shared" si="6"/>
-        <v>370.80000000000018</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17">
+        <v>93.242469958545072</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="8"/>
+        <v>0.32098881460591328</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="7"/>
+        <v>320.98881460591326</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="9"/>
+        <v>307.87608005179959</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20">
       <c r="B21">
         <v>127</v>
       </c>
@@ -4026,10 +4180,22 @@
       </c>
       <c r="Q21">
         <f t="shared" si="6"/>
-        <v>423</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17">
+        <v>100.62521269448108</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="8"/>
+        <v>0.33700721193054178</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="7"/>
+        <v>337.00721193054176</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="9"/>
+        <v>328.82003107573166</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20">
       <c r="B22">
         <v>138</v>
       </c>
@@ -4074,10 +4240,22 @@
       </c>
       <c r="Q22">
         <f t="shared" si="6"/>
-        <v>424.79999999999927</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17">
+        <v>108.039371356953</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="8"/>
+        <v>0.27161686484161685</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="7"/>
+        <v>271.61686484161686</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="9"/>
+        <v>302.89050910153748</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20">
       <c r="B23">
         <v>148</v>
       </c>
@@ -4122,10 +4300,22 @@
       </c>
       <c r="Q23">
         <f t="shared" si="6"/>
-        <v>373.5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17">
+        <v>114.5581761131518</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="8"/>
+        <v>0.30869562596143213</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="7"/>
+        <v>308.69562596143214</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="9"/>
+        <v>289.76179049599455</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20">
       <c r="B24">
         <v>158</v>
       </c>
@@ -4170,10 +4360,22 @@
       </c>
       <c r="Q24">
         <f t="shared" si="6"/>
-        <v>406.80000000000018</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17">
+        <v>121.65817551026474</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="8"/>
+        <v>0.32915323029656723</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="7"/>
+        <v>329.15323029656724</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="9"/>
+        <v>318.69712141416483</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20">
       <c r="B25">
         <v>168</v>
       </c>
@@ -4218,10 +4420,22 @@
       </c>
       <c r="Q25">
         <f t="shared" si="6"/>
-        <v>414.90000000000055</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17">
+        <v>128.89954657678922</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="8"/>
+        <v>0.28994282198755766</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="7"/>
+        <v>289.94282198755764</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="9"/>
+        <v>308.6956259614318</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20">
       <c r="B26">
         <v>179</v>
       </c>
@@ -4266,10 +4480,22 @@
       </c>
       <c r="Q26">
         <f t="shared" si="6"/>
-        <v>398.69999999999982</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17">
+        <v>135.8581743044906</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="8"/>
+        <v>0.32772523363584583</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="7"/>
+        <v>327.72523363584583</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="9"/>
+        <v>308.01267103673894</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20">
       <c r="B27">
         <v>191</v>
       </c>
@@ -4314,10 +4540,22 @@
       </c>
       <c r="Q27">
         <f t="shared" si="6"/>
-        <v>413.10000000000036</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17">
+        <v>143.06812944447921</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="8"/>
+        <v>0.28820697822062807</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="7"/>
+        <v>288.20697822062806</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="9"/>
+        <v>307.52701420140124</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20">
       <c r="B28">
         <v>202</v>
       </c>
@@ -4362,10 +4600,22 @@
       </c>
       <c r="Q28">
         <f t="shared" si="6"/>
-        <v>379.79999999999927</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17">
+        <v>149.69688994355366</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="8"/>
+        <v>0.3262972369751212</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="7"/>
+        <v>326.29723697512122</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="9"/>
+        <v>306.82888250060245</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20">
       <c r="B29">
         <v>213</v>
       </c>
@@ -4410,10 +4660,22 @@
       </c>
       <c r="Q29">
         <f t="shared" si="6"/>
-        <v>411.30000000000109</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17">
+        <v>156.87542915700632</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="8"/>
+        <v>0.31074449073551341</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="7"/>
+        <v>310.74449073551341</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="9"/>
+        <v>318.34805556376608</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20">
       <c r="B30">
         <v>225</v>
       </c>
@@ -4458,10 +4720,22 @@
       </c>
       <c r="Q30">
         <f t="shared" si="6"/>
-        <v>409.5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17">
+        <v>164.02255244392313</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="8"/>
+        <v>0.26908424032921097</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="7"/>
+        <v>269.08424032921096</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="9"/>
+        <v>289.91436553236224</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20">
       <c r="B31">
         <v>236</v>
       </c>
@@ -4506,10 +4780,22 @@
       </c>
       <c r="Q31">
         <f t="shared" si="6"/>
-        <v>354.59999999999854</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17">
+        <v>170.21148997149498</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="8"/>
+        <v>0.30630528372500621</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="7"/>
+        <v>306.30528372500623</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="9"/>
+        <v>288.09073057387235</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20">
       <c r="B32">
         <v>247</v>
       </c>
@@ -4554,10 +4840,22 @@
       </c>
       <c r="Q32">
         <f t="shared" si="6"/>
-        <v>421.20000000000073</v>
-      </c>
-    </row>
-    <row r="33" spans="2:17">
+        <v>177.56281678089513</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="8"/>
+        <v>0.32415524198403678</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="7"/>
+        <v>324.15524198403676</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="9"/>
+        <v>314.84222028367304</v>
+      </c>
+    </row>
+    <row r="33" spans="2:20">
       <c r="B33">
         <v>259</v>
       </c>
@@ -4602,10 +4900,22 @@
       </c>
       <c r="Q33">
         <f t="shared" si="6"/>
-        <v>408.60000000000036</v>
-      </c>
-    </row>
-    <row r="34" spans="2:17">
+        <v>184.69423210454394</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="8"/>
+        <v>0.28601583117056961</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="7"/>
+        <v>286.01583117056964</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="9"/>
+        <v>304.25641895092349</v>
+      </c>
+    </row>
+    <row r="34" spans="2:20">
       <c r="B34">
         <v>271</v>
       </c>
@@ -4650,10 +4960,22 @@
       </c>
       <c r="Q34">
         <f t="shared" si="6"/>
-        <v>393.29999999999927</v>
-      </c>
-    </row>
-    <row r="35" spans="2:17">
+        <v>191.55861205263761</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="8"/>
+        <v>0.33200922361801327</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="7"/>
+        <v>332.00922361801327</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="9"/>
+        <v>308.01267103673837</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20">
       <c r="B35">
         <v>282</v>
       </c>
@@ -4698,10 +5020,22 @@
       </c>
       <c r="Q35">
         <f t="shared" si="6"/>
-        <v>418.5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:17">
+        <v>198.86281497223391</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="8"/>
+        <v>0.26572637861613657</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="7"/>
+        <v>265.72637861613657</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="9"/>
+        <v>297.42686970399069</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20">
       <c r="B36">
         <v>293</v>
       </c>
@@ -4746,10 +5080,22 @@
       </c>
       <c r="Q36">
         <f t="shared" si="6"/>
-        <v>365.39999999999964</v>
-      </c>
-    </row>
-    <row r="37" spans="2:17">
+        <v>205.24024805902118</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="8"/>
+        <v>0.32781836385284735</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="7"/>
+        <v>327.81836385284737</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="9"/>
+        <v>296.11181820005891</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20">
       <c r="B37">
         <v>305</v>
       </c>
@@ -4794,10 +5140,22 @@
       </c>
       <c r="Q37">
         <f t="shared" si="6"/>
-        <v>432</v>
-      </c>
-    </row>
-    <row r="38" spans="2:17">
+        <v>212.78007042763667</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="8"/>
+        <v>0.31006153581081902</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="7"/>
+        <v>310.06153581081901</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="9"/>
+        <v>318.93994983183319</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20">
       <c r="B38">
         <v>316</v>
       </c>
@@ -4842,10 +5200,22 @@
       </c>
       <c r="Q38">
         <f t="shared" si="6"/>
-        <v>408.60000000000036</v>
-      </c>
-    </row>
-    <row r="39" spans="2:17">
+        <v>219.91148575128551</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="8"/>
+        <v>0.28863382504856244</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="7"/>
+        <v>288.63382504856241</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="9"/>
+        <v>299.1197260598795</v>
+      </c>
+    </row>
+    <row r="39" spans="2:20">
       <c r="B39">
         <v>328</v>
       </c>
@@ -4890,10 +5260,22 @@
       </c>
       <c r="Q39">
         <f t="shared" si="6"/>
-        <v>396.89999999999964</v>
-      </c>
-    </row>
-    <row r="40" spans="2:17">
+        <v>226.83869755245101</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="8"/>
+        <v>0.32843923196620556</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="7"/>
+        <v>328.43923196620557</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="9"/>
+        <v>307.67119357439179</v>
+      </c>
+    </row>
+    <row r="40" spans="2:20">
       <c r="B40">
         <v>339</v>
       </c>
@@ -4938,10 +5320,22 @@
       </c>
       <c r="Q40">
         <f t="shared" si="6"/>
-        <v>414</v>
-      </c>
-    </row>
-    <row r="41" spans="2:17">
+        <v>234.06436065570753</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="8"/>
+        <v>0.26899887096362579</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="7"/>
+        <v>268.99887096362579</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="9"/>
+        <v>297.42686970399001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:20">
       <c r="B41">
         <v>351</v>
       </c>
@@ -4986,10 +5380,22 @@
       </c>
       <c r="Q41">
         <f t="shared" si="6"/>
-        <v>369.90000000000146</v>
-      </c>
-    </row>
-    <row r="42" spans="2:17">
+        <v>240.52033355883455</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="8"/>
+        <v>0.32772523363584455</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="7"/>
+        <v>327.72523363584457</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="9"/>
+        <v>297.08539224164349</v>
+      </c>
+    </row>
+    <row r="42" spans="2:20">
       <c r="B42">
         <v>362</v>
       </c>
@@ -5034,10 +5440,22 @@
       </c>
       <c r="Q42">
         <f t="shared" si="6"/>
-        <v>413.09999999999854</v>
-      </c>
-    </row>
-    <row r="43" spans="2:17">
+        <v>247.73028869882313</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="8"/>
+        <v>0.30041479749952416</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="7"/>
+        <v>300.41479749952418</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="9"/>
+        <v>313.47631043428606</v>
+      </c>
+    </row>
+    <row r="43" spans="2:20">
       <c r="B43">
         <v>373</v>
       </c>
@@ -5082,10 +5500,22 @@
       </c>
       <c r="Q43">
         <f t="shared" si="6"/>
-        <v>413.10000000000036</v>
-      </c>
-    </row>
-    <row r="44" spans="2:17">
+        <v>254.94024383881171</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="8"/>
+        <v>0.31344526702861875</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="7"/>
+        <v>313.44526702861873</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="9"/>
+        <v>306.64676118735201</v>
+      </c>
+    </row>
+    <row r="44" spans="2:20">
       <c r="B44">
         <v>385</v>
       </c>
@@ -5130,10 +5560,22 @@
       </c>
       <c r="Q44">
         <f t="shared" si="6"/>
-        <v>395.10000000000036</v>
-      </c>
-    </row>
-    <row r="45" spans="2:17">
+        <v>261.83603971344132</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="8"/>
+        <v>0.30434178831651099</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="7"/>
+        <v>304.34178831651099</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="9"/>
+        <v>308.69562596143214</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20">
       <c r="B45">
         <v>397</v>
       </c>
@@ -5178,10 +5620,22 @@
       </c>
       <c r="Q45">
         <f t="shared" si="6"/>
-        <v>418.5</v>
-      </c>
-    </row>
-    <row r="46" spans="2:17">
+        <v>269.14024263303759</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="8"/>
+        <v>0.2841092486724679</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="7"/>
+        <v>284.10924867246791</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="9"/>
+        <v>294.44075827793671</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20">
       <c r="B46">
         <v>408</v>
       </c>
@@ -5226,10 +5680,22 @@
       </c>
       <c r="Q46">
         <f t="shared" si="6"/>
-        <v>374.39999999999964</v>
-      </c>
-    </row>
-    <row r="47" spans="2:17">
+        <v>275.67475535250435</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="8"/>
+        <v>0.30630528372500504</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="7"/>
+        <v>306.30528372500504</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="9"/>
+        <v>295.44339423121022</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20">
       <c r="B47">
         <v>419</v>
       </c>
@@ -5274,10 +5740,22 @@
       </c>
       <c r="Q47">
         <f t="shared" si="6"/>
-        <v>421.20000000000073</v>
-      </c>
-    </row>
-    <row r="48" spans="2:17">
+        <v>283.02608216190447</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="8"/>
+        <v>0.29913425701572477</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="7"/>
+        <v>299.13425701572476</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="9"/>
+        <v>302.79605788854872</v>
+      </c>
+    </row>
+    <row r="48" spans="2:20">
       <c r="B48">
         <v>430</v>
       </c>
@@ -5322,10 +5800,22 @@
       </c>
       <c r="Q48">
         <f t="shared" si="6"/>
-        <v>394.20000000000073</v>
-      </c>
-    </row>
-    <row r="49" spans="2:17">
+        <v>289.90617007326614</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="8"/>
+        <v>0.3189399498318326</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="7"/>
+        <v>318.93994983183262</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="9"/>
+        <v>309.03710342377872</v>
+      </c>
+    </row>
+    <row r="49" spans="2:20">
       <c r="B49">
         <v>442</v>
       </c>
@@ -5370,10 +5860,22 @@
       </c>
       <c r="Q49">
         <f t="shared" si="6"/>
-        <v>420.29999999999927</v>
-      </c>
-    </row>
-    <row r="50" spans="2:17">
+        <v>297.24178891939829</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="8"/>
+        <v>0.30565078525550621</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="7"/>
+        <v>305.65078525550621</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="9"/>
+        <v>312.15399345243191</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20">
       <c r="B50">
         <v>454</v>
       </c>
@@ -5418,10 +5920,22 @@
       </c>
       <c r="Q50">
         <f t="shared" si="6"/>
-        <v>420.29999999999927</v>
-      </c>
-    </row>
-    <row r="51" spans="2:17">
+        <v>304.57740776553044</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="8"/>
+        <v>0.29981721194041916</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="7"/>
+        <v>299.81721194041916</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="9"/>
+        <v>302.79605788854872</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20">
       <c r="B51">
         <v>465</v>
       </c>
@@ -5466,10 +5980,22 @@
       </c>
       <c r="Q51">
         <f t="shared" si="6"/>
-        <v>395.10000000000218</v>
-      </c>
-    </row>
-    <row r="52" spans="2:17">
+        <v>311.47320364016008</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="8"/>
+        <v>0.30368728984701221</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="7"/>
+        <v>303.68728984701221</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="9"/>
+        <v>301.79342193527521</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20">
       <c r="B52">
         <v>477</v>
       </c>
@@ -5514,10 +6040,22 @@
       </c>
       <c r="Q52">
         <f t="shared" si="6"/>
-        <v>417.59999999999854</v>
-      </c>
-    </row>
-    <row r="53" spans="2:17">
+        <v>318.76169859648837</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="8"/>
+        <v>0.28342629374777595</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="7"/>
+        <v>283.42629374777596</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="9"/>
+        <v>293.77233430908808</v>
+      </c>
+    </row>
+    <row r="53" spans="2:20">
       <c r="B53">
         <v>488</v>
       </c>
@@ -5562,10 +6100,22 @@
       </c>
       <c r="Q53">
         <f t="shared" si="6"/>
-        <v>373.5</v>
-      </c>
-    </row>
-    <row r="54" spans="2:17">
+        <v>325.28050335268722</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="8"/>
+        <v>0.32576949907876662</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="7"/>
+        <v>325.76949907876661</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="9"/>
+        <v>304.59789641327126</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20">
       <c r="B54">
         <v>499</v>
       </c>
@@ -5610,10 +6160,22 @@
       </c>
       <c r="Q54">
         <f t="shared" si="6"/>
-        <v>429.29999999999927</v>
-      </c>
-    </row>
-    <row r="55" spans="2:17">
+        <v>332.77320183149885</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="8"/>
+        <v>0.30391494148857567</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="7"/>
+        <v>303.91494148857566</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="9"/>
+        <v>314.84222028367117</v>
+      </c>
+    </row>
+    <row r="55" spans="2:20">
       <c r="B55">
         <v>510</v>
       </c>
@@ -5658,10 +6220,22 @@
       </c>
       <c r="Q55">
         <f t="shared" si="6"/>
-        <v>400.5</v>
-      </c>
-    </row>
-    <row r="56" spans="2:17">
+        <v>339.76324548573609</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="8"/>
+        <v>0.29779680362153488</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="7"/>
+        <v>297.79680362153488</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="9"/>
+        <v>300.79078598200164</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20">
       <c r="B56">
         <v>523</v>
       </c>
@@ -5706,10 +6280,22 @@
       </c>
       <c r="Q56">
         <f t="shared" si="6"/>
-        <v>409.5</v>
-      </c>
-    </row>
-    <row r="57" spans="2:17">
+        <v>346.91036877265293</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="8"/>
+        <v>0.31484222028367115</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="7"/>
+        <v>314.84222028367117</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="9"/>
+        <v>306.13817773279305</v>
+      </c>
+    </row>
+    <row r="57" spans="2:20">
       <c r="B57">
         <v>534</v>
       </c>
@@ -5754,10 +6340,22 @@
       </c>
       <c r="Q57">
         <f t="shared" si="6"/>
-        <v>414.90000000000146</v>
-      </c>
-    </row>
-    <row r="58" spans="2:17">
+        <v>354.15173983917737</v>
+      </c>
+      <c r="R57">
+        <f t="shared" si="8"/>
+        <v>0.28012534494509111</v>
+      </c>
+      <c r="S57">
+        <f t="shared" si="7"/>
+        <v>280.12534494509111</v>
+      </c>
+      <c r="T57">
+        <f t="shared" si="9"/>
+        <v>297.11445415333242</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20">
       <c r="B58">
         <v>545</v>
       </c>
@@ -5802,10 +6400,22 @@
       </c>
       <c r="Q58">
         <f t="shared" si="6"/>
-        <v>385.20000000000073</v>
-      </c>
-    </row>
-    <row r="59" spans="2:17">
+        <v>360.87474811785955</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="8"/>
+        <v>0.30303279137751576</v>
+      </c>
+      <c r="S58">
+        <f t="shared" si="7"/>
+        <v>303.03279137751576</v>
+      </c>
+      <c r="T58">
+        <f t="shared" si="9"/>
+        <v>291.57906816130344</v>
+      </c>
+    </row>
+    <row r="59" spans="2:20">
       <c r="B59">
         <v>556</v>
       </c>
@@ -5850,10 +6460,22 @@
       </c>
       <c r="Q59">
         <f t="shared" si="6"/>
-        <v>416.69999999999709</v>
-      </c>
-    </row>
-    <row r="60" spans="2:17">
+        <v>368.14753511091993</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="8"/>
+        <v>0.30059329708211374</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="7"/>
+        <v>300.59329708211374</v>
+      </c>
+      <c r="T59">
+        <f t="shared" si="9"/>
+        <v>301.86607671449747</v>
+      </c>
+    </row>
+    <row r="60" spans="2:20">
       <c r="B60">
         <v>569</v>
       </c>
@@ -5898,10 +6520,22 @@
       </c>
       <c r="Q60">
         <f t="shared" si="6"/>
-        <v>378.90000000000146</v>
-      </c>
-    </row>
-    <row r="61" spans="2:17">
+        <v>374.76058764672644</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="8"/>
+        <v>0.3121957699504847</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="7"/>
+        <v>312.1957699504847</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="9"/>
+        <v>306.64676118735082</v>
+      </c>
+    </row>
+    <row r="61" spans="2:20">
       <c r="B61">
         <v>582</v>
       </c>
@@ -5946,10 +6580,22 @@
       </c>
       <c r="Q61">
         <f t="shared" si="6"/>
-        <v>429.29999999999927</v>
-      </c>
-    </row>
-    <row r="62" spans="2:17">
+        <v>382.25328612553807</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="8"/>
+        <v>0.30664676118735323</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="7"/>
+        <v>306.64676118735321</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="9"/>
+        <v>309.48029757703739</v>
+      </c>
+    </row>
+    <row r="62" spans="2:20">
       <c r="B62">
         <v>594</v>
       </c>
@@ -5994,10 +6640,22 @@
       </c>
       <c r="Q62">
         <f t="shared" si="6"/>
-        <v>404.10000000000218</v>
-      </c>
-    </row>
-    <row r="63" spans="2:17">
+        <v>389.30616163284719</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="8"/>
+        <v>0.29648780668253494</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="7"/>
+        <v>296.48780668253494</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="9"/>
+        <v>301.45920995085027</v>
+      </c>
+    </row>
+    <row r="63" spans="2:20">
       <c r="B63">
         <v>607</v>
       </c>
@@ -6042,10 +6700,22 @@
       </c>
       <c r="Q63">
         <f t="shared" si="6"/>
-        <v>407.69999999999709</v>
-      </c>
-    </row>
-    <row r="64" spans="2:17">
+        <v>396.42186899322803</v>
+      </c>
+      <c r="R63">
+        <f t="shared" si="8"/>
+        <v>0.31893994983183754</v>
+      </c>
+      <c r="S63">
+        <f t="shared" si="7"/>
+        <v>318.93994983183757</v>
+      </c>
+      <c r="T63">
+        <f t="shared" si="9"/>
+        <v>307.4750256704915</v>
+      </c>
+    </row>
+    <row r="64" spans="2:20">
       <c r="B64">
         <v>619</v>
       </c>
@@ -6090,10 +6760,22 @@
       </c>
       <c r="Q64">
         <f t="shared" si="6"/>
-        <v>420.30000000000291</v>
-      </c>
-    </row>
-    <row r="65" spans="2:17">
+        <v>403.75748783936029</v>
+      </c>
+      <c r="R64">
+        <f t="shared" si="8"/>
+        <v>0.27423485871960435</v>
+      </c>
+      <c r="S64">
+        <f t="shared" si="7"/>
+        <v>274.23485871960435</v>
+      </c>
+      <c r="T64">
+        <f t="shared" si="9"/>
+        <v>296.11181820005891</v>
+      </c>
+    </row>
+    <row r="65" spans="2:20">
       <c r="B65">
         <v>631</v>
       </c>
@@ -6138,10 +6820,22 @@
       </c>
       <c r="Q65">
         <f t="shared" si="6"/>
-        <v>377.09999999999854</v>
-      </c>
-    </row>
-    <row r="66" spans="2:17">
+        <v>410.3391244486308</v>
+      </c>
+      <c r="R65">
+        <f t="shared" si="8"/>
+        <v>0.32629723697512375</v>
+      </c>
+      <c r="S65">
+        <f t="shared" si="7"/>
+        <v>326.29723697512372</v>
+      </c>
+      <c r="T65">
+        <f t="shared" si="9"/>
+        <v>299.13425701572231</v>
+      </c>
+    </row>
+    <row r="66" spans="2:20">
       <c r="B66">
         <v>644</v>
       </c>
@@ -6186,10 +6880,22 @@
       </c>
       <c r="Q66">
         <f t="shared" si="6"/>
-        <v>411.29999999999927</v>
-      </c>
-    </row>
-    <row r="67" spans="2:17">
+        <v>417.51766366208352</v>
+      </c>
+      <c r="R66">
+        <f t="shared" si="8"/>
+        <v>0.27750735106710067</v>
+      </c>
+      <c r="S66">
+        <f t="shared" si="7"/>
+        <v>277.50735106710067</v>
+      </c>
+      <c r="T66">
+        <f t="shared" si="9"/>
+        <v>300.84164432745951</v>
+      </c>
+    </row>
+    <row r="67" spans="2:20">
       <c r="B67">
         <v>657</v>
       </c>
@@ -6234,10 +6940,22 @@
       </c>
       <c r="Q67">
         <f t="shared" si="6"/>
-        <v>381.60000000000218</v>
-      </c>
-    </row>
-    <row r="68" spans="2:17">
+        <v>424.17784008769394</v>
+      </c>
+      <c r="R67">
+        <f t="shared" si="8"/>
+        <v>0.3102322745419907</v>
+      </c>
+      <c r="S67">
+        <f t="shared" si="7"/>
+        <v>310.23227454199071</v>
+      </c>
+      <c r="T67">
+        <f t="shared" si="9"/>
+        <v>293.86981280454569</v>
+      </c>
+    </row>
+    <row r="68" spans="2:20">
       <c r="B68">
         <v>669</v>
       </c>
@@ -6282,10 +7000,22 @@
       </c>
       <c r="Q68">
         <f t="shared" si="6"/>
-        <v>426.59999999999854</v>
-      </c>
-    </row>
-    <row r="69" spans="2:17">
+        <v>431.62341467670171</v>
+      </c>
+      <c r="R68">
+        <f t="shared" si="8"/>
+        <v>0.31279335550959292</v>
+      </c>
+      <c r="S68">
+        <f t="shared" si="7"/>
+        <v>312.79335550959291</v>
+      </c>
+      <c r="T68">
+        <f t="shared" si="9"/>
+        <v>311.48556948358322</v>
+      </c>
+    </row>
+    <row r="69" spans="2:20">
       <c r="B69">
         <v>681</v>
       </c>
@@ -6330,10 +7060,22 @@
       </c>
       <c r="Q69">
         <f t="shared" si="6"/>
-        <v>412.20000000000073</v>
-      </c>
-    </row>
-    <row r="70" spans="2:17">
+        <v>438.81766185342235</v>
+      </c>
+      <c r="R69">
+        <f t="shared" si="8"/>
+        <v>0.29059732045705289</v>
+      </c>
+      <c r="S69">
+        <f t="shared" si="7"/>
+        <v>290.59732045705289</v>
+      </c>
+      <c r="T69">
+        <f t="shared" si="9"/>
+        <v>301.45920995084907</v>
+      </c>
+    </row>
+    <row r="70" spans="2:20">
       <c r="B70">
         <v>694</v>
       </c>
@@ -6341,7 +7083,7 @@
         <v>15413</v>
       </c>
       <c r="D70">
-        <f t="shared" ref="D70:D103" si="7">C71-C70</f>
+        <f t="shared" ref="D70:D103" si="10">C71-C70</f>
         <v>500</v>
       </c>
       <c r="F70">
@@ -6351,15 +7093,15 @@
         <v>23484</v>
       </c>
       <c r="H70">
-        <f t="shared" ref="H70:H87" si="8">G71-G70</f>
+        <f t="shared" ref="H70:H87" si="11">G71-G70</f>
         <v>498</v>
       </c>
       <c r="I70">
-        <f t="shared" ref="I70:I88" si="9">G70*1.8/2</f>
+        <f t="shared" ref="I70:I88" si="12">G70*1.8/2</f>
         <v>21135.600000000002</v>
       </c>
       <c r="J70">
-        <f t="shared" ref="J70:J87" si="10">I71-I70</f>
+        <f t="shared" ref="J70:J87" si="13">I71-I70</f>
         <v>448.19999999999709</v>
       </c>
       <c r="M70">
@@ -6369,19 +7111,31 @@
         <v>28380</v>
       </c>
       <c r="O70">
-        <f t="shared" ref="O70:O79" si="11">M70-143</f>
+        <f t="shared" ref="O70:O79" si="14">M70-143</f>
         <v>1481</v>
       </c>
       <c r="P70">
-        <f t="shared" ref="P70:P79" si="12">N70*1.8/2</f>
+        <f t="shared" ref="P70:P79" si="15">N70*1.8/2</f>
         <v>25542</v>
       </c>
       <c r="Q70">
-        <f t="shared" si="6"/>
-        <v>399.59999999999854</v>
-      </c>
-    </row>
-    <row r="71" spans="2:17">
+        <f t="shared" ref="Q70:Q79" si="16">P70*PI()/180</f>
+        <v>445.79199754439162</v>
+      </c>
+      <c r="R70">
+        <f t="shared" ref="R70:R78" si="17">(Q71-Q70)/(M71-M70)</f>
+        <v>0.33415121860909641</v>
+      </c>
+      <c r="S70">
+        <f t="shared" ref="S70:S78" si="18">R70*1000</f>
+        <v>334.15121860909642</v>
+      </c>
+      <c r="T70">
+        <f t="shared" si="9"/>
+        <v>311.42744566020411</v>
+      </c>
+    </row>
+    <row r="71" spans="2:20">
       <c r="B71">
         <v>706</v>
       </c>
@@ -6389,7 +7143,7 @@
         <v>15913</v>
       </c>
       <c r="D71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>498</v>
       </c>
       <c r="F71">
@@ -6399,15 +7153,15 @@
         <v>23982</v>
       </c>
       <c r="H71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>500</v>
       </c>
       <c r="I71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>21583.8</v>
       </c>
       <c r="J71">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>450</v>
       </c>
       <c r="M71">
@@ -6417,19 +7171,31 @@
         <v>28848</v>
       </c>
       <c r="O71">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1503</v>
       </c>
       <c r="P71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>25963.200000000001</v>
       </c>
       <c r="Q71">
-        <f t="shared" ref="Q71:Q78" si="13">P71-P70</f>
-        <v>421.20000000000073</v>
-      </c>
-    </row>
-    <row r="72" spans="2:17">
+        <f t="shared" si="16"/>
+        <v>453.14332435379174</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="17"/>
+        <v>0.27096236637211746</v>
+      </c>
+      <c r="S71">
+        <f t="shared" si="18"/>
+        <v>270.96236637211746</v>
+      </c>
+      <c r="T71">
+        <f t="shared" ref="T71:T78" si="19">(Q72-Q70)/(M72-M70)*1000</f>
+        <v>301.18312178980307</v>
+      </c>
+    </row>
+    <row r="72" spans="2:20">
       <c r="B72">
         <v>719</v>
       </c>
@@ -6437,7 +7203,7 @@
         <v>16411</v>
       </c>
       <c r="D72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>490</v>
       </c>
       <c r="F72">
@@ -6447,15 +7213,15 @@
         <v>24482</v>
       </c>
       <c r="H72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>496</v>
       </c>
       <c r="I72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>22033.8</v>
       </c>
       <c r="J72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>446.40000000000146</v>
       </c>
       <c r="M72">
@@ -6465,19 +7231,31 @@
         <v>29262</v>
       </c>
       <c r="O72">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1527</v>
       </c>
       <c r="P72">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>26335.8</v>
       </c>
       <c r="Q72">
-        <f t="shared" si="13"/>
-        <v>372.59999999999854</v>
-      </c>
-    </row>
-    <row r="73" spans="2:17">
+        <f t="shared" si="16"/>
+        <v>459.64642114672256</v>
+      </c>
+      <c r="R72">
+        <f t="shared" si="17"/>
+        <v>0.31552517520837048</v>
+      </c>
+      <c r="S72">
+        <f t="shared" si="18"/>
+        <v>315.52517520837046</v>
+      </c>
+      <c r="T72">
+        <f t="shared" si="19"/>
+        <v>292.76969835581571</v>
+      </c>
+    </row>
+    <row r="73" spans="2:20">
       <c r="B73">
         <v>732</v>
       </c>
@@ -6485,7 +7263,7 @@
         <v>16901</v>
       </c>
       <c r="D73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>498</v>
       </c>
       <c r="F73">
@@ -6495,15 +7273,15 @@
         <v>24978</v>
       </c>
       <c r="H73">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>496</v>
       </c>
       <c r="I73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>22480.2</v>
       </c>
       <c r="J73">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>446.40000000000146</v>
       </c>
       <c r="M73">
@@ -6513,19 +7291,31 @@
         <v>29724</v>
       </c>
       <c r="O73">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1550</v>
       </c>
       <c r="P73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>26751.600000000002</v>
       </c>
       <c r="Q73">
-        <f t="shared" si="13"/>
-        <v>415.80000000000291</v>
-      </c>
-    </row>
-    <row r="74" spans="2:17">
+        <f t="shared" si="16"/>
+        <v>466.90350017651508</v>
+      </c>
+      <c r="R73">
+        <f t="shared" si="17"/>
+        <v>0.27881634800609351</v>
+      </c>
+      <c r="S73">
+        <f t="shared" si="18"/>
+        <v>278.81634800609351</v>
+      </c>
+      <c r="T73">
+        <f t="shared" si="19"/>
+        <v>296.78024216890992</v>
+      </c>
+    </row>
+    <row r="74" spans="2:20">
       <c r="B74">
         <v>744</v>
       </c>
@@ -6533,7 +7323,7 @@
         <v>17399</v>
       </c>
       <c r="D74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>488</v>
       </c>
       <c r="F74">
@@ -6543,15 +7333,15 @@
         <v>25474</v>
       </c>
       <c r="H74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>504</v>
       </c>
       <c r="I74">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>22926.600000000002</v>
       </c>
       <c r="J74">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>453.59999999999854</v>
       </c>
       <c r="M74">
@@ -6561,19 +7351,31 @@
         <v>30150</v>
       </c>
       <c r="O74">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1574</v>
       </c>
       <c r="P74">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>27135</v>
       </c>
       <c r="Q74">
-        <f t="shared" si="13"/>
-        <v>383.39999999999782</v>
-      </c>
-    </row>
-    <row r="75" spans="2:17">
+        <f t="shared" si="16"/>
+        <v>473.59509252866133</v>
+      </c>
+      <c r="R74">
+        <f t="shared" si="17"/>
+        <v>0.3196229047565245</v>
+      </c>
+      <c r="S74">
+        <f t="shared" si="18"/>
+        <v>319.62290475652452</v>
+      </c>
+      <c r="T74">
+        <f t="shared" si="19"/>
+        <v>298.78551407545336</v>
+      </c>
+    </row>
+    <row r="75" spans="2:20">
       <c r="B75">
         <v>756</v>
       </c>
@@ -6581,7 +7383,7 @@
         <v>17887</v>
       </c>
       <c r="D75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>498</v>
       </c>
       <c r="F75">
@@ -6591,15 +7393,15 @@
         <v>25978</v>
       </c>
       <c r="H75">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>498</v>
       </c>
       <c r="I75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>23380.2</v>
       </c>
       <c r="J75">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>448.20000000000073</v>
       </c>
       <c r="M75">
@@ -6609,19 +7411,31 @@
         <v>30618</v>
       </c>
       <c r="O75">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1597</v>
       </c>
       <c r="P75">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>27556.2</v>
       </c>
       <c r="Q75">
-        <f t="shared" si="13"/>
-        <v>421.20000000000073</v>
-      </c>
-    </row>
-    <row r="76" spans="2:17">
+        <f t="shared" si="16"/>
+        <v>480.94641933806139</v>
+      </c>
+      <c r="R75">
+        <f t="shared" si="17"/>
+        <v>0.30237829290801699</v>
+      </c>
+      <c r="S75">
+        <f t="shared" si="18"/>
+        <v>302.37829290801699</v>
+      </c>
+      <c r="T75">
+        <f t="shared" si="19"/>
+        <v>310.81714551473345</v>
+      </c>
+    </row>
+    <row r="76" spans="2:20">
       <c r="B76">
         <v>768</v>
       </c>
@@ -6629,7 +7443,7 @@
         <v>18385</v>
       </c>
       <c r="D76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>496</v>
       </c>
       <c r="F76">
@@ -6639,15 +7453,15 @@
         <v>26476</v>
       </c>
       <c r="H76">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>498</v>
       </c>
       <c r="I76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>23828.400000000001</v>
       </c>
       <c r="J76">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>448.20000000000073</v>
       </c>
       <c r="M76">
@@ -6657,19 +7471,31 @@
         <v>31080</v>
       </c>
       <c r="O76">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1621</v>
       </c>
       <c r="P76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>27972</v>
       </c>
       <c r="Q76">
-        <f t="shared" si="13"/>
-        <v>415.79999999999927</v>
-      </c>
-    </row>
-    <row r="77" spans="2:17">
+        <f t="shared" si="16"/>
+        <v>488.2034983678538</v>
+      </c>
+      <c r="R76">
+        <f t="shared" si="17"/>
+        <v>0.29776834716634093</v>
+      </c>
+      <c r="S76">
+        <f t="shared" si="18"/>
+        <v>297.7683471663409</v>
+      </c>
+      <c r="T76">
+        <f t="shared" si="19"/>
+        <v>300.12236201315426</v>
+      </c>
+    </row>
+    <row r="77" spans="2:20">
       <c r="B77">
         <v>782</v>
       </c>
@@ -6677,7 +7503,7 @@
         <v>18881</v>
       </c>
       <c r="D77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>490</v>
       </c>
       <c r="F77">
@@ -6687,15 +7513,15 @@
         <v>26974</v>
       </c>
       <c r="H77">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>498</v>
       </c>
       <c r="I77">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>24276.600000000002</v>
       </c>
       <c r="J77">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>448.19999999999709</v>
       </c>
       <c r="M77">
@@ -6705,19 +7531,31 @@
         <v>31516</v>
       </c>
       <c r="O77">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1644</v>
       </c>
       <c r="P77">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>28364.400000000001</v>
       </c>
       <c r="Q77">
-        <f t="shared" si="13"/>
-        <v>392.40000000000146</v>
-      </c>
-    </row>
-    <row r="78" spans="2:17">
+        <f t="shared" si="16"/>
+        <v>495.05217035267964</v>
+      </c>
+      <c r="R77">
+        <f t="shared" si="17"/>
+        <v>0.3100615358108178</v>
+      </c>
+      <c r="S77">
+        <f t="shared" si="18"/>
+        <v>310.06153581081782</v>
+      </c>
+      <c r="T77">
+        <f t="shared" si="19"/>
+        <v>303.91494148857942</v>
+      </c>
+    </row>
+    <row r="78" spans="2:20">
       <c r="B78">
         <v>794</v>
       </c>
@@ -6725,7 +7563,7 @@
         <v>19371</v>
       </c>
       <c r="D78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
       <c r="F78">
@@ -6735,15 +7573,15 @@
         <v>27472</v>
       </c>
       <c r="H78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>500</v>
       </c>
       <c r="I78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>24724.799999999999</v>
       </c>
       <c r="J78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>450</v>
       </c>
       <c r="M78">
@@ -6753,19 +7591,31 @@
         <v>31970</v>
       </c>
       <c r="O78">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1667</v>
       </c>
       <c r="P78">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>28773</v>
       </c>
       <c r="Q78">
-        <f t="shared" si="13"/>
-        <v>408.59999999999854</v>
-      </c>
-    </row>
-    <row r="79" spans="2:17">
+        <f t="shared" si="16"/>
+        <v>502.18358567632845</v>
+      </c>
+      <c r="R78">
+        <f t="shared" si="17"/>
+        <v>0.28143434188408395</v>
+      </c>
+      <c r="S78">
+        <f t="shared" si="18"/>
+        <v>281.43434188408395</v>
+      </c>
+      <c r="T78">
+        <f t="shared" si="19"/>
+        <v>295.44339423120903</v>
+      </c>
+    </row>
+    <row r="79" spans="2:20">
       <c r="B79">
         <v>806</v>
       </c>
@@ -6773,7 +7623,7 @@
         <v>19875</v>
       </c>
       <c r="D79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>488</v>
       </c>
       <c r="F79">
@@ -6783,15 +7633,15 @@
         <v>27972</v>
       </c>
       <c r="H79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>502</v>
       </c>
       <c r="I79">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>25174.799999999999</v>
       </c>
       <c r="J79">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>451.80000000000291</v>
       </c>
       <c r="M79">
@@ -6801,15 +7651,19 @@
         <v>32400</v>
       </c>
       <c r="O79">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1691</v>
       </c>
       <c r="P79">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>29160</v>
       </c>
-    </row>
-    <row r="80" spans="2:17">
+      <c r="Q79">
+        <f t="shared" si="16"/>
+        <v>508.93800988154646</v>
+      </c>
+    </row>
+    <row r="80" spans="2:20">
       <c r="B80">
         <v>819</v>
       </c>
@@ -6817,7 +7671,7 @@
         <v>20363</v>
       </c>
       <c r="D80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>500</v>
       </c>
       <c r="F80">
@@ -6827,15 +7681,15 @@
         <v>28474</v>
       </c>
       <c r="H80">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>506</v>
       </c>
       <c r="I80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>25626.600000000002</v>
       </c>
       <c r="J80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>455.39999999999782</v>
       </c>
     </row>
@@ -6847,7 +7701,7 @@
         <v>20863</v>
       </c>
       <c r="D81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
       <c r="F81">
@@ -6857,15 +7711,15 @@
         <v>28980</v>
       </c>
       <c r="H81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>494</v>
       </c>
       <c r="I81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>26082</v>
       </c>
       <c r="J81">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>444.60000000000218</v>
       </c>
     </row>
@@ -6877,7 +7731,7 @@
         <v>21367</v>
       </c>
       <c r="D82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
       <c r="F82">
@@ -6887,15 +7741,15 @@
         <v>29474</v>
       </c>
       <c r="H82">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>498</v>
       </c>
       <c r="I82">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>26526.600000000002</v>
       </c>
       <c r="J82">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>448.19999999999709</v>
       </c>
     </row>
@@ -6907,7 +7761,7 @@
         <v>21871</v>
       </c>
       <c r="D83">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
       <c r="F83">
@@ -6917,15 +7771,15 @@
         <v>29972</v>
       </c>
       <c r="H83">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>498</v>
       </c>
       <c r="I83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>26974.799999999999</v>
       </c>
       <c r="J83">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>448.20000000000073</v>
       </c>
     </row>
@@ -6937,7 +7791,7 @@
         <v>22375</v>
       </c>
       <c r="D84">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
       <c r="F84">
@@ -6947,15 +7801,15 @@
         <v>30470</v>
       </c>
       <c r="H84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>500</v>
       </c>
       <c r="I84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>27423</v>
       </c>
       <c r="J84">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>450</v>
       </c>
     </row>
@@ -6967,7 +7821,7 @@
         <v>22879</v>
       </c>
       <c r="D85">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>476</v>
       </c>
       <c r="F85">
@@ -6977,15 +7831,15 @@
         <v>30970</v>
       </c>
       <c r="H85">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>492</v>
       </c>
       <c r="I85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>27873</v>
       </c>
       <c r="J85">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>442.79999999999927</v>
       </c>
     </row>
@@ -6997,7 +7851,7 @@
         <v>23355</v>
       </c>
       <c r="D86">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
       <c r="F86">
@@ -7007,15 +7861,15 @@
         <v>31462</v>
       </c>
       <c r="H86">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>508</v>
       </c>
       <c r="I86">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>28315.8</v>
       </c>
       <c r="J86">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>457.20000000000073</v>
       </c>
     </row>
@@ -7027,7 +7881,7 @@
         <v>23859</v>
       </c>
       <c r="D87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
       <c r="F87">
@@ -7037,15 +7891,15 @@
         <v>31970</v>
       </c>
       <c r="H87">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>494</v>
       </c>
       <c r="I87">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>28773</v>
       </c>
       <c r="J87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>444.60000000000218</v>
       </c>
     </row>
@@ -7057,7 +7911,7 @@
         <v>24363</v>
       </c>
       <c r="D88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
       <c r="F88">
@@ -7067,7 +7921,7 @@
         <v>32464</v>
       </c>
       <c r="I88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>29217.600000000002</v>
       </c>
     </row>
@@ -7079,7 +7933,7 @@
         <v>24867</v>
       </c>
       <c r="D89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
     </row>
@@ -7091,7 +7945,7 @@
         <v>25371</v>
       </c>
       <c r="D90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
     </row>
@@ -7103,7 +7957,7 @@
         <v>25875</v>
       </c>
       <c r="D91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>504</v>
       </c>
     </row>
@@ -7115,7 +7969,7 @@
         <v>26379</v>
       </c>
       <c r="D92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>502</v>
       </c>
     </row>
@@ -7127,7 +7981,7 @@
         <v>26881</v>
       </c>
       <c r="D93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>464</v>
       </c>
     </row>
@@ -7139,7 +7993,7 @@
         <v>27345</v>
       </c>
       <c r="D94">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>508</v>
       </c>
     </row>
@@ -7151,7 +8005,7 @@
         <v>27853</v>
       </c>
       <c r="D95">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>506</v>
       </c>
     </row>
@@ -7163,7 +8017,7 @@
         <v>28359</v>
       </c>
       <c r="D96">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>508</v>
       </c>
     </row>
@@ -7175,7 +8029,7 @@
         <v>28867</v>
       </c>
       <c r="D97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>494</v>
       </c>
     </row>
@@ -7187,7 +8041,7 @@
         <v>29361</v>
       </c>
       <c r="D98">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>508</v>
       </c>
     </row>
@@ -7199,7 +8053,7 @@
         <v>29869</v>
       </c>
       <c r="D99">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>506</v>
       </c>
     </row>
@@ -7211,7 +8065,7 @@
         <v>30375</v>
       </c>
       <c r="D100">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>532</v>
       </c>
     </row>
@@ -7223,7 +8077,7 @@
         <v>30907</v>
       </c>
       <c r="D101">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>540</v>
       </c>
     </row>
@@ -7235,7 +8089,7 @@
         <v>31447</v>
       </c>
       <c r="D102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>548</v>
       </c>
     </row>
@@ -7247,7 +8101,7 @@
         <v>31995</v>
       </c>
       <c r="D103">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>544</v>
       </c>
     </row>

</xml_diff>